<commit_message>
1. DynamicExcelGenerator.java runs dynamic actions ( by ItemLargeBox props )
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="17">
   <si>
     <t/>
   </si>
@@ -23,13 +23,20 @@
     <t>Photo of element</t>
   </si>
   <si>
-    <t>#REF!</t>
+    <t>Саморезы гипс/металл
+3.5x25</t>
   </si>
   <si>
     <t>Marking</t>
   </si>
   <si>
+    <t>YZP</t>
+  </si>
+  <si>
     <t>РАЗМЕР/Size</t>
+  </si>
+  <si>
+    <t>3.5x25</t>
   </si>
   <si>
     <t>Кол-во/Q-ty</t>
@@ -39,6 +46,9 @@
   </si>
   <si>
     <t>Кол-во в упак/шт.</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
   <si>
     <t>Вес упак Кг/Kgs</t>
@@ -51,6 +61,9 @@
   </si>
   <si>
     <t>ORDER:</t>
+  </si>
+  <si>
+    <t>2155695PL</t>
   </si>
 </sst>
 </file>
@@ -2110,7 +2123,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s" s="3">
         <v>0</v>
@@ -2119,7 +2132,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s" s="7">
         <v>0</v>
@@ -2128,7 +2141,7 @@
         <v>4</v>
       </c>
       <c r="K5" t="s" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5" t="s" s="11">
         <v>0</v>
@@ -2137,7 +2150,7 @@
         <v>4</v>
       </c>
       <c r="O5" t="s" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P5" t="s" s="15">
         <v>0</v>
@@ -2146,7 +2159,7 @@
         <v>4</v>
       </c>
       <c r="S5" t="s" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T5" t="s" s="19">
         <v>0</v>
@@ -2155,7 +2168,7 @@
         <v>4</v>
       </c>
       <c r="W5" t="s" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X5" t="s" s="23">
         <v>0</v>
@@ -2164,7 +2177,7 @@
         <v>4</v>
       </c>
       <c r="AA5" t="s" s="27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB5" t="s" s="27">
         <v>0</v>
@@ -2173,7 +2186,7 @@
         <v>4</v>
       </c>
       <c r="AE5" t="s" s="31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AF5" t="s" s="31">
         <v>0</v>
@@ -2182,7 +2195,7 @@
         <v>4</v>
       </c>
       <c r="AI5" t="s" s="35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AJ5" t="s" s="35">
         <v>0</v>
@@ -2191,7 +2204,7 @@
         <v>4</v>
       </c>
       <c r="AM5" t="s" s="39">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AN5" t="s" s="39">
         <v>0</v>
@@ -2200,7 +2213,7 @@
         <v>4</v>
       </c>
       <c r="AQ5" t="s" s="43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AR5" t="s" s="43">
         <v>0</v>
@@ -2209,7 +2222,7 @@
         <v>4</v>
       </c>
       <c r="AU5" t="s" s="47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AV5" t="s" s="47">
         <v>0</v>
@@ -2218,7 +2231,7 @@
         <v>4</v>
       </c>
       <c r="AY5" t="s" s="51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AZ5" t="s" s="51">
         <v>0</v>
@@ -2227,7 +2240,7 @@
         <v>4</v>
       </c>
       <c r="BC5" t="s" s="55">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BD5" t="s" s="55">
         <v>0</v>
@@ -2236,7 +2249,7 @@
         <v>4</v>
       </c>
       <c r="BG5" t="s" s="59">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BH5" t="s" s="59">
         <v>0</v>
@@ -2245,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="BK5" t="s" s="63">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BL5" t="s" s="63">
         <v>0</v>
@@ -2254,7 +2267,7 @@
         <v>4</v>
       </c>
       <c r="BO5" t="s" s="67">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BP5" t="s" s="67">
         <v>0</v>
@@ -2263,7 +2276,7 @@
         <v>4</v>
       </c>
       <c r="BS5" t="s" s="71">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BT5" t="s" s="71">
         <v>0</v>
@@ -2272,7 +2285,7 @@
         <v>4</v>
       </c>
       <c r="BW5" t="s" s="75">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BX5" t="s" s="75">
         <v>0</v>
@@ -2281,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="CA5" t="s" s="79">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CB5" t="s" s="79">
         <v>0</v>
@@ -2290,7 +2303,7 @@
         <v>4</v>
       </c>
       <c r="CE5" t="s" s="83">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CF5" t="s" s="83">
         <v>0</v>
@@ -2299,7 +2312,7 @@
         <v>4</v>
       </c>
       <c r="CI5" t="s" s="87">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CJ5" t="s" s="87">
         <v>0</v>
@@ -2308,7 +2321,7 @@
         <v>4</v>
       </c>
       <c r="CM5" t="s" s="91">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CN5" t="s" s="91">
         <v>0</v>
@@ -2317,7 +2330,7 @@
         <v>4</v>
       </c>
       <c r="CQ5" t="s" s="95">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CR5" t="s" s="95">
         <v>0</v>
@@ -2326,7 +2339,7 @@
         <v>4</v>
       </c>
       <c r="CU5" t="s" s="99">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CV5" t="s" s="99">
         <v>0</v>
@@ -2335,7 +2348,7 @@
         <v>4</v>
       </c>
       <c r="CY5" t="s" s="103">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CZ5" t="s" s="103">
         <v>0</v>
@@ -2344,7 +2357,7 @@
         <v>4</v>
       </c>
       <c r="DC5" t="s" s="107">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="DD5" t="s" s="107">
         <v>0</v>
@@ -2353,7 +2366,7 @@
         <v>4</v>
       </c>
       <c r="DG5" t="s" s="111">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="DH5" t="s" s="111">
         <v>0</v>
@@ -2362,7 +2375,7 @@
         <v>4</v>
       </c>
       <c r="DK5" t="s" s="115">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="DL5" t="s" s="115">
         <v>0</v>
@@ -2371,7 +2384,7 @@
         <v>4</v>
       </c>
       <c r="DO5" t="s" s="119">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="DP5" t="s" s="119">
         <v>0</v>
@@ -2379,271 +2392,271 @@
     </row>
     <row r="6">
       <c r="B6" t="s" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s" s="3">
         <v>0</v>
       </c>
       <c r="F6" t="s" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s" s="7">
         <v>0</v>
       </c>
       <c r="J6" t="s" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s" s="11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L6" t="s" s="11">
         <v>0</v>
       </c>
       <c r="N6" t="s" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O6" t="s" s="15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="P6" t="s" s="15">
         <v>0</v>
       </c>
       <c r="R6" t="s" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S6" t="s" s="19">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="T6" t="s" s="19">
         <v>0</v>
       </c>
       <c r="V6" t="s" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W6" t="s" s="23">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X6" t="s" s="23">
         <v>0</v>
       </c>
       <c r="Z6" t="s" s="28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AA6" t="s" s="27">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AB6" t="s" s="27">
         <v>0</v>
       </c>
       <c r="AD6" t="s" s="32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AE6" t="s" s="31">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AF6" t="s" s="31">
         <v>0</v>
       </c>
       <c r="AH6" t="s" s="36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI6" t="s" s="35">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AJ6" t="s" s="35">
         <v>0</v>
       </c>
       <c r="AL6" t="s" s="40">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AM6" t="s" s="39">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AN6" t="s" s="39">
         <v>0</v>
       </c>
       <c r="AP6" t="s" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AQ6" t="s" s="43">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AR6" t="s" s="43">
         <v>0</v>
       </c>
       <c r="AT6" t="s" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AU6" t="s" s="47">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AV6" t="s" s="47">
         <v>0</v>
       </c>
       <c r="AX6" t="s" s="52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AY6" t="s" s="51">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AZ6" t="s" s="51">
         <v>0</v>
       </c>
       <c r="BB6" t="s" s="56">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BC6" t="s" s="55">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BD6" t="s" s="55">
         <v>0</v>
       </c>
       <c r="BF6" t="s" s="60">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BG6" t="s" s="59">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BH6" t="s" s="59">
         <v>0</v>
       </c>
       <c r="BJ6" t="s" s="64">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BK6" t="s" s="63">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BL6" t="s" s="63">
         <v>0</v>
       </c>
       <c r="BN6" t="s" s="68">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BO6" t="s" s="67">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BP6" t="s" s="67">
         <v>0</v>
       </c>
       <c r="BR6" t="s" s="72">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BS6" t="s" s="71">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BT6" t="s" s="71">
         <v>0</v>
       </c>
       <c r="BV6" t="s" s="76">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BW6" t="s" s="75">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BX6" t="s" s="75">
         <v>0</v>
       </c>
       <c r="BZ6" t="s" s="80">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CA6" t="s" s="79">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CB6" t="s" s="79">
         <v>0</v>
       </c>
       <c r="CD6" t="s" s="84">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CE6" t="s" s="83">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CF6" t="s" s="83">
         <v>0</v>
       </c>
       <c r="CH6" t="s" s="88">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CI6" t="s" s="87">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CJ6" t="s" s="87">
         <v>0</v>
       </c>
       <c r="CL6" t="s" s="92">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CM6" t="s" s="91">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CN6" t="s" s="91">
         <v>0</v>
       </c>
       <c r="CP6" t="s" s="96">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CQ6" t="s" s="95">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CR6" t="s" s="95">
         <v>0</v>
       </c>
       <c r="CT6" t="s" s="100">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CU6" t="s" s="99">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CV6" t="s" s="99">
         <v>0</v>
       </c>
       <c r="CX6" t="s" s="104">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CY6" t="s" s="103">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="CZ6" t="s" s="103">
         <v>0</v>
       </c>
       <c r="DB6" t="s" s="108">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="DC6" t="s" s="107">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="DD6" t="s" s="107">
         <v>0</v>
       </c>
       <c r="DF6" t="s" s="112">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="DG6" t="s" s="111">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="DH6" t="s" s="111">
         <v>0</v>
       </c>
       <c r="DJ6" t="s" s="116">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="DK6" t="s" s="115">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="DL6" t="s" s="115">
         <v>0</v>
       </c>
       <c r="DN6" t="s" s="120">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="DO6" t="s" s="119">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="DP6" t="s" s="119">
         <v>0</v>
@@ -2651,818 +2664,818 @@
     </row>
     <row r="7">
       <c r="B7" t="s" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s" s="3">
         <v>0</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s" s="7">
         <v>0</v>
       </c>
       <c r="H7" t="s" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J7" t="s" s="12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K7" t="s" s="11">
         <v>0</v>
       </c>
       <c r="L7" t="s" s="12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N7" t="s" s="16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O7" t="s" s="15">
         <v>0</v>
       </c>
       <c r="P7" t="s" s="16">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R7" t="s" s="20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S7" t="s" s="19">
         <v>0</v>
       </c>
       <c r="T7" t="s" s="20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V7" t="s" s="24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W7" t="s" s="23">
         <v>0</v>
       </c>
       <c r="X7" t="s" s="24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Z7" t="s" s="28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AA7" t="s" s="27">
         <v>0</v>
       </c>
       <c r="AB7" t="s" s="28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AD7" t="s" s="32">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AE7" t="s" s="31">
         <v>0</v>
       </c>
       <c r="AF7" t="s" s="32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AH7" t="s" s="36">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AI7" t="s" s="35">
         <v>0</v>
       </c>
       <c r="AJ7" t="s" s="36">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AL7" t="s" s="40">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AM7" t="s" s="39">
         <v>0</v>
       </c>
       <c r="AN7" t="s" s="40">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AP7" t="s" s="44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AQ7" t="s" s="43">
         <v>0</v>
       </c>
       <c r="AR7" t="s" s="44">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AT7" t="s" s="48">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AU7" t="s" s="47">
         <v>0</v>
       </c>
       <c r="AV7" t="s" s="48">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AX7" t="s" s="52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AY7" t="s" s="51">
         <v>0</v>
       </c>
       <c r="AZ7" t="s" s="52">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BB7" t="s" s="56">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BC7" t="s" s="55">
         <v>0</v>
       </c>
       <c r="BD7" t="s" s="56">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BF7" t="s" s="60">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BG7" t="s" s="59">
         <v>0</v>
       </c>
       <c r="BH7" t="s" s="60">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BJ7" t="s" s="64">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BK7" t="s" s="63">
         <v>0</v>
       </c>
       <c r="BL7" t="s" s="64">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BN7" t="s" s="68">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BO7" t="s" s="67">
         <v>0</v>
       </c>
       <c r="BP7" t="s" s="68">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BR7" t="s" s="72">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BS7" t="s" s="71">
         <v>0</v>
       </c>
       <c r="BT7" t="s" s="72">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BV7" t="s" s="76">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BW7" t="s" s="75">
         <v>0</v>
       </c>
       <c r="BX7" t="s" s="76">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BZ7" t="s" s="80">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CA7" t="s" s="79">
         <v>0</v>
       </c>
       <c r="CB7" t="s" s="80">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CD7" t="s" s="84">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CE7" t="s" s="83">
         <v>0</v>
       </c>
       <c r="CF7" t="s" s="84">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CH7" t="s" s="88">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CI7" t="s" s="87">
         <v>0</v>
       </c>
       <c r="CJ7" t="s" s="88">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CL7" t="s" s="92">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CM7" t="s" s="91">
         <v>0</v>
       </c>
       <c r="CN7" t="s" s="92">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CP7" t="s" s="96">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CQ7" t="s" s="95">
         <v>0</v>
       </c>
       <c r="CR7" t="s" s="96">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CT7" t="s" s="100">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CU7" t="s" s="99">
         <v>0</v>
       </c>
       <c r="CV7" t="s" s="100">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CX7" t="s" s="104">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CY7" t="s" s="103">
         <v>0</v>
       </c>
       <c r="CZ7" t="s" s="104">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DB7" t="s" s="108">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="DC7" t="s" s="107">
         <v>0</v>
       </c>
       <c r="DD7" t="s" s="108">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DF7" t="s" s="112">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="DG7" t="s" s="111">
         <v>0</v>
       </c>
       <c r="DH7" t="s" s="112">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DJ7" t="s" s="116">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="DK7" t="s" s="115">
         <v>0</v>
       </c>
       <c r="DL7" t="s" s="116">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DN7" t="s" s="120">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="DO7" t="s" s="119">
         <v>0</v>
       </c>
       <c r="DP7" t="s" s="120">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s" s="7">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J8" t="s" s="12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K8" t="s" s="11">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="L8" t="s" s="12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N8" t="s" s="16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O8" t="s" s="15">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="P8" t="s" s="16">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R8" t="s" s="20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S8" t="s" s="19">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="T8" t="s" s="20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V8" t="s" s="24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="W8" t="s" s="23">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="X8" t="s" s="24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Z8" t="s" s="28">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AA8" t="s" s="27">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AB8" t="s" s="28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AD8" t="s" s="32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AE8" t="s" s="31">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AF8" t="s" s="32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AH8" t="s" s="36">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AI8" t="s" s="35">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AJ8" t="s" s="36">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AL8" t="s" s="40">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AM8" t="s" s="39">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AN8" t="s" s="40">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AP8" t="s" s="44">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AQ8" t="s" s="43">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AR8" t="s" s="44">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AT8" t="s" s="48">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AU8" t="s" s="47">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AV8" t="s" s="48">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AX8" t="s" s="52">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AY8" t="s" s="51">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AZ8" t="s" s="52">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BB8" t="s" s="56">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BC8" t="s" s="55">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="BD8" t="s" s="56">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BF8" t="s" s="60">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BG8" t="s" s="59">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="BH8" t="s" s="60">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BJ8" t="s" s="64">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BK8" t="s" s="63">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="BL8" t="s" s="64">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BN8" t="s" s="68">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BO8" t="s" s="67">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="BP8" t="s" s="68">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BR8" t="s" s="72">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BS8" t="s" s="71">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="BT8" t="s" s="72">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BV8" t="s" s="76">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BW8" t="s" s="75">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="BX8" t="s" s="76">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BZ8" t="s" s="80">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="CA8" t="s" s="79">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="CB8" t="s" s="80">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CD8" t="s" s="84">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="CE8" t="s" s="83">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="CF8" t="s" s="84">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CH8" t="s" s="88">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="CI8" t="s" s="87">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="CJ8" t="s" s="88">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CL8" t="s" s="92">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="CM8" t="s" s="91">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="CN8" t="s" s="92">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CP8" t="s" s="96">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="CQ8" t="s" s="95">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="CR8" t="s" s="96">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CT8" t="s" s="100">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="CU8" t="s" s="99">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="CV8" t="s" s="100">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CX8" t="s" s="104">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="CY8" t="s" s="103">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="CZ8" t="s" s="104">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DB8" t="s" s="108">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="DC8" t="s" s="107">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="DD8" t="s" s="108">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DF8" t="s" s="112">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="DG8" t="s" s="111">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="DH8" t="s" s="112">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DJ8" t="s" s="116">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="DK8" t="s" s="115">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="DL8" t="s" s="116">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DN8" t="s" s="120">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="DO8" t="s" s="119">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="DP8" t="s" s="120">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s" s="3">
         <v>0</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s" s="7">
         <v>0</v>
       </c>
       <c r="H9" t="s" s="8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s" s="12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K9" t="s" s="11">
         <v>0</v>
       </c>
       <c r="L9" t="s" s="12">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N9" t="s" s="16">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O9" t="s" s="15">
         <v>0</v>
       </c>
       <c r="P9" t="s" s="16">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="R9" t="s" s="20">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S9" t="s" s="19">
         <v>0</v>
       </c>
       <c r="T9" t="s" s="20">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="V9" t="s" s="24">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="W9" t="s" s="23">
         <v>0</v>
       </c>
       <c r="X9" t="s" s="24">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Z9" t="s" s="28">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AA9" t="s" s="27">
         <v>0</v>
       </c>
       <c r="AB9" t="s" s="28">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AD9" t="s" s="32">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AE9" t="s" s="31">
         <v>0</v>
       </c>
       <c r="AF9" t="s" s="32">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AH9" t="s" s="36">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AI9" t="s" s="35">
         <v>0</v>
       </c>
       <c r="AJ9" t="s" s="36">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AL9" t="s" s="40">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AM9" t="s" s="39">
         <v>0</v>
       </c>
       <c r="AN9" t="s" s="40">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AP9" t="s" s="44">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AQ9" t="s" s="43">
         <v>0</v>
       </c>
       <c r="AR9" t="s" s="44">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AT9" t="s" s="48">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AU9" t="s" s="47">
         <v>0</v>
       </c>
       <c r="AV9" t="s" s="48">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AX9" t="s" s="52">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AY9" t="s" s="51">
         <v>0</v>
       </c>
       <c r="AZ9" t="s" s="52">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BB9" t="s" s="56">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BC9" t="s" s="55">
         <v>0</v>
       </c>
       <c r="BD9" t="s" s="56">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BF9" t="s" s="60">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BG9" t="s" s="59">
         <v>0</v>
       </c>
       <c r="BH9" t="s" s="60">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BJ9" t="s" s="64">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BK9" t="s" s="63">
         <v>0</v>
       </c>
       <c r="BL9" t="s" s="64">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BN9" t="s" s="68">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BO9" t="s" s="67">
         <v>0</v>
       </c>
       <c r="BP9" t="s" s="68">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BR9" t="s" s="72">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BS9" t="s" s="71">
         <v>0</v>
       </c>
       <c r="BT9" t="s" s="72">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BV9" t="s" s="76">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BW9" t="s" s="75">
         <v>0</v>
       </c>
       <c r="BX9" t="s" s="76">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="BZ9" t="s" s="80">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="CA9" t="s" s="79">
         <v>0</v>
       </c>
       <c r="CB9" t="s" s="80">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="CD9" t="s" s="84">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="CE9" t="s" s="83">
         <v>0</v>
       </c>
       <c r="CF9" t="s" s="84">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="CH9" t="s" s="88">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="CI9" t="s" s="87">
         <v>0</v>
       </c>
       <c r="CJ9" t="s" s="88">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="CL9" t="s" s="92">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="CM9" t="s" s="91">
         <v>0</v>
       </c>
       <c r="CN9" t="s" s="92">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="CP9" t="s" s="96">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="CQ9" t="s" s="95">
         <v>0</v>
       </c>
       <c r="CR9" t="s" s="96">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="CT9" t="s" s="100">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="CU9" t="s" s="99">
         <v>0</v>
       </c>
       <c r="CV9" t="s" s="100">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="CX9" t="s" s="104">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="CY9" t="s" s="103">
         <v>0</v>
       </c>
       <c r="CZ9" t="s" s="104">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="DB9" t="s" s="108">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="DC9" t="s" s="107">
         <v>0</v>
       </c>
       <c r="DD9" t="s" s="108">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="DF9" t="s" s="112">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="DG9" t="s" s="111">
         <v>0</v>
       </c>
       <c r="DH9" t="s" s="112">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="DJ9" t="s" s="116">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="DK9" t="s" s="115">
         <v>0</v>
       </c>
       <c r="DL9" t="s" s="116">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="DN9" t="s" s="120">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="DO9" t="s" s="119">
         <v>0</v>
       </c>
       <c r="DP9" t="s" s="120">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -3470,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s" s="4">
         <v>0</v>
@@ -3479,7 +3492,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s" s="8">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s" s="8">
         <v>0</v>
@@ -3488,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s" s="12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L10" t="s" s="12">
         <v>0</v>
@@ -3497,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="O10" t="s" s="16">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="P10" t="s" s="16">
         <v>0</v>
@@ -3506,7 +3519,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="s" s="20">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="T10" t="s" s="20">
         <v>0</v>
@@ -3515,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="W10" t="s" s="24">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="X10" t="s" s="24">
         <v>0</v>
@@ -3524,7 +3537,7 @@
         <v>0</v>
       </c>
       <c r="AA10" t="s" s="28">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AB10" t="s" s="28">
         <v>0</v>
@@ -3533,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="AE10" t="s" s="32">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AF10" t="s" s="32">
         <v>0</v>
@@ -3542,7 +3555,7 @@
         <v>0</v>
       </c>
       <c r="AI10" t="s" s="36">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AJ10" t="s" s="36">
         <v>0</v>
@@ -3551,7 +3564,7 @@
         <v>0</v>
       </c>
       <c r="AM10" t="s" s="40">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AN10" t="s" s="40">
         <v>0</v>
@@ -3560,7 +3573,7 @@
         <v>0</v>
       </c>
       <c r="AQ10" t="s" s="44">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AR10" t="s" s="44">
         <v>0</v>
@@ -3569,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="AU10" t="s" s="48">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AV10" t="s" s="48">
         <v>0</v>
@@ -3578,7 +3591,7 @@
         <v>0</v>
       </c>
       <c r="AY10" t="s" s="52">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AZ10" t="s" s="52">
         <v>0</v>
@@ -3587,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="BC10" t="s" s="56">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BD10" t="s" s="56">
         <v>0</v>
@@ -3596,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="BG10" t="s" s="60">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BH10" t="s" s="60">
         <v>0</v>
@@ -3605,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="BK10" t="s" s="64">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BL10" t="s" s="64">
         <v>0</v>
@@ -3614,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="BO10" t="s" s="68">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BP10" t="s" s="68">
         <v>0</v>
@@ -3623,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="BS10" t="s" s="72">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BT10" t="s" s="72">
         <v>0</v>
@@ -3632,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="BW10" t="s" s="76">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BX10" t="s" s="76">
         <v>0</v>
@@ -3641,7 +3654,7 @@
         <v>0</v>
       </c>
       <c r="CA10" t="s" s="80">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="CB10" t="s" s="80">
         <v>0</v>
@@ -3650,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="CE10" t="s" s="84">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="CF10" t="s" s="84">
         <v>0</v>
@@ -3659,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="CI10" t="s" s="88">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="CJ10" t="s" s="88">
         <v>0</v>
@@ -3668,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="CM10" t="s" s="92">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="CN10" t="s" s="92">
         <v>0</v>
@@ -3677,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="CQ10" t="s" s="96">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="CR10" t="s" s="96">
         <v>0</v>
@@ -3686,7 +3699,7 @@
         <v>0</v>
       </c>
       <c r="CU10" t="s" s="100">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="CV10" t="s" s="100">
         <v>0</v>
@@ -3695,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="CY10" t="s" s="104">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="CZ10" t="s" s="104">
         <v>0</v>
@@ -3704,7 +3717,7 @@
         <v>0</v>
       </c>
       <c r="DC10" t="s" s="108">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="DD10" t="s" s="108">
         <v>0</v>
@@ -3713,7 +3726,7 @@
         <v>0</v>
       </c>
       <c r="DG10" t="s" s="112">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="DH10" t="s" s="112">
         <v>0</v>
@@ -3722,7 +3735,7 @@
         <v>0</v>
       </c>
       <c r="DK10" t="s" s="116">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="DL10" t="s" s="116">
         <v>0</v>
@@ -3731,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="DO10" t="s" s="120">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="DP10" t="s" s="120">
         <v>0</v>
@@ -3739,271 +3752,271 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s" s="4">
         <v>0</v>
       </c>
       <c r="F11" t="s" s="8">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s" s="8">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s" s="8">
         <v>0</v>
       </c>
       <c r="J11" t="s" s="12">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K11" t="s" s="12">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="L11" t="s" s="12">
         <v>0</v>
       </c>
       <c r="N11" t="s" s="16">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O11" t="s" s="16">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="P11" t="s" s="16">
         <v>0</v>
       </c>
       <c r="R11" t="s" s="20">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="S11" t="s" s="20">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="T11" t="s" s="20">
         <v>0</v>
       </c>
       <c r="V11" t="s" s="24">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="W11" t="s" s="24">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="X11" t="s" s="24">
         <v>0</v>
       </c>
       <c r="Z11" t="s" s="28">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AA11" t="s" s="28">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AB11" t="s" s="28">
         <v>0</v>
       </c>
       <c r="AD11" t="s" s="32">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AE11" t="s" s="32">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AF11" t="s" s="32">
         <v>0</v>
       </c>
       <c r="AH11" t="s" s="36">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AI11" t="s" s="36">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AJ11" t="s" s="36">
         <v>0</v>
       </c>
       <c r="AL11" t="s" s="40">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AM11" t="s" s="40">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AN11" t="s" s="40">
         <v>0</v>
       </c>
       <c r="AP11" t="s" s="44">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AQ11" t="s" s="44">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AR11" t="s" s="44">
         <v>0</v>
       </c>
       <c r="AT11" t="s" s="48">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AU11" t="s" s="48">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AV11" t="s" s="48">
         <v>0</v>
       </c>
       <c r="AX11" t="s" s="52">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AY11" t="s" s="52">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AZ11" t="s" s="52">
         <v>0</v>
       </c>
       <c r="BB11" t="s" s="56">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BC11" t="s" s="56">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="BD11" t="s" s="56">
         <v>0</v>
       </c>
       <c r="BF11" t="s" s="60">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BG11" t="s" s="60">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="BH11" t="s" s="60">
         <v>0</v>
       </c>
       <c r="BJ11" t="s" s="64">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BK11" t="s" s="64">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="BL11" t="s" s="64">
         <v>0</v>
       </c>
       <c r="BN11" t="s" s="68">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BO11" t="s" s="68">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="BP11" t="s" s="68">
         <v>0</v>
       </c>
       <c r="BR11" t="s" s="72">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BS11" t="s" s="72">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="BT11" t="s" s="72">
         <v>0</v>
       </c>
       <c r="BV11" t="s" s="76">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="BW11" t="s" s="76">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="BX11" t="s" s="76">
         <v>0</v>
       </c>
       <c r="BZ11" t="s" s="80">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="CA11" t="s" s="80">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="CB11" t="s" s="80">
         <v>0</v>
       </c>
       <c r="CD11" t="s" s="84">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="CE11" t="s" s="84">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="CF11" t="s" s="84">
         <v>0</v>
       </c>
       <c r="CH11" t="s" s="88">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="CI11" t="s" s="88">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="CJ11" t="s" s="88">
         <v>0</v>
       </c>
       <c r="CL11" t="s" s="92">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="CM11" t="s" s="92">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="CN11" t="s" s="92">
         <v>0</v>
       </c>
       <c r="CP11" t="s" s="96">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="CQ11" t="s" s="96">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="CR11" t="s" s="96">
         <v>0</v>
       </c>
       <c r="CT11" t="s" s="100">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="CU11" t="s" s="100">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="CV11" t="s" s="100">
         <v>0</v>
       </c>
       <c r="CX11" t="s" s="104">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="CY11" t="s" s="104">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="CZ11" t="s" s="104">
         <v>0</v>
       </c>
       <c r="DB11" t="s" s="108">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="DC11" t="s" s="108">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="DD11" t="s" s="108">
         <v>0</v>
       </c>
       <c r="DF11" t="s" s="112">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="DG11" t="s" s="112">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="DH11" t="s" s="112">
         <v>0</v>
       </c>
       <c r="DJ11" t="s" s="116">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="DK11" t="s" s="116">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="DL11" t="s" s="116">
         <v>0</v>
       </c>
       <c r="DN11" t="s" s="120">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="DO11" t="s" s="120">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="DP11" t="s" s="120">
         <v>0</v>

</xml_diff>